<commit_message>
Update land use files
</commit_message>
<xml_diff>
--- a/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
+++ b/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jonah\Documents\EPS Model\.eps-oregon-1.4.3.2 - WIP\InputData\land\AOCoLUPpUA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-oregon\InputData\land\AOCoLUPpUA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E524E63C-9F1E-4C87-AEBE-1731DFC63BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1688CFB5-FDC6-4858-ADCF-456B73CBE5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6480" windowWidth="15990" windowHeight="24990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,15 @@
   <definedNames>
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>AOCoLUPpUA Annual Ongoing Cost of Land Use Policies per Unit Area</t>
   </si>
@@ -225,9 +228,6 @@
   </si>
   <si>
     <t>Calculated Average Forest Management Cost (Just PNW)</t>
-  </si>
-  <si>
-    <t>2017$ / acre</t>
   </si>
   <si>
     <t>Adjusting to 2017 dollars using "cpi.xlsx" in the InputData folder.</t>
@@ -804,14 +804,14 @@
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -819,98 +819,97 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2006</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1.278</v>
       </c>
@@ -918,37 +917,37 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1.06765</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -964,26 +963,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
@@ -994,7 +993,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>25879</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>25349</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1033,7 +1032,7 @@
         <v>52050</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1046,7 +1045,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1059,7 +1058,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1072,7 +1071,7 @@
         <v>2574</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>2688</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1098,7 +1097,7 @@
         <v>59869</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>35138</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -1119,7 +1118,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1143,7 +1142,7 @@
       </c>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1156,7 +1155,7 @@
         <v>3.5460000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1170,7 +1169,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1185,7 +1184,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1196,12 +1195,12 @@
         <v>58.48</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1214,7 +1213,7 @@
         <v>1.671</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1228,7 +1227,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1239,7 +1238,7 @@
         <v>14.82</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1250,12 +1249,12 @@
         <v>58.48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1268,7 +1267,7 @@
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1282,7 +1281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>14.82</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1304,12 +1303,12 @@
         <v>58.48</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1322,7 +1321,7 @@
         <v>3.7700000000000005</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>39</v>
       </c>
@@ -1338,7 +1337,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>41</v>
       </c>
@@ -1354,7 +1353,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>43</v>
       </c>
@@ -1370,19 +1369,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
         <f>(SUM(B16:B19)*B7+SUM(C16:C19)*C7)/SUM(B7:C7)</f>
         <v>177.68697307584281</v>
@@ -1391,7 +1390,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
         <f>A39*About!A27</f>
         <v>227.08395159092711</v>
@@ -1400,14 +1399,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
-        <f>A40*About!A35</f>
-        <v>242.44618091605332</v>
-      </c>
-      <c r="B41" t="s">
-        <v>63</v>
-      </c>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1426,12 +1419,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1444,8 +1437,8 @@
         <v>9</v>
       </c>
       <c r="B2" s="3">
-        <f>'Forest Mgmt Costs'!A41</f>
-        <v>242.44618091605332</v>
+        <f>'Forest Mgmt Costs'!A40</f>
+        <v>227.08395159092711</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1453,8 +1446,8 @@
         <v>10</v>
       </c>
       <c r="B3" s="3">
-        <f>'Forest Mgmt Costs'!A41</f>
-        <v>242.44618091605332</v>
+        <f>'Forest Mgmt Costs'!A40</f>
+        <v>227.08395159092711</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1470,7 +1463,8 @@
         <v>12</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <f>'Forest Mgmt Costs'!A40</f>
+        <v>227.08395159092711</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Align LULUCF potential and policies with Graves et al study
</commit_message>
<xml_diff>
--- a/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
+++ b/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-oregon\InputData\land\AOCoLUPpUA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1688CFB5-FDC6-4858-ADCF-456B73CBE5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E36E8C-04F4-455C-92C7-032BE1EFFC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>AOCoLUPpUA Annual Ongoing Cost of Land Use Policies per Unit Area</t>
   </si>
@@ -56,18 +56,6 @@
     <t>avoid emission of sequestered CO2.</t>
   </si>
   <si>
-    <t>This variable is NOT for use with the Improved Forest Management policy,</t>
-  </si>
-  <si>
-    <t>as that policy must be repeated every year in order to obtain carbon benefits</t>
-  </si>
-  <si>
-    <t>in that year.  Its cost is handled in the "Implementation Cost of Land Use</t>
-  </si>
-  <si>
-    <t>Policies per Unit Area" variable.</t>
-  </si>
-  <si>
     <t>forest set asides</t>
   </si>
   <si>
@@ -89,12 +77,6 @@
     <t>annual maintenance cost ($ / acre)</t>
   </si>
   <si>
-    <t>Avoid deforestion, peatland restoration, and forest restoration policies</t>
-  </si>
-  <si>
-    <t>are not used in the U.S. version of the model.</t>
-  </si>
-  <si>
     <t>land use policies (such as "Afforestation/Reforestation") and thereby</t>
   </si>
   <si>
@@ -234,6 +216,15 @@
   </si>
   <si>
     <t>2012 to 2017</t>
+  </si>
+  <si>
+    <t>Forest management is not used in the Oregon EPS.</t>
+  </si>
+  <si>
+    <t>Due to lack of data, we do not include costs for the "peatland restoration" policy, which</t>
+  </si>
+  <si>
+    <t>we map to sagebrush conservation.</t>
   </si>
 </sst>
 </file>
@@ -798,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,7 +807,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -826,17 +817,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -846,108 +837,93 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>17</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>57</v>
+      <c r="A22" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>1.278</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>1.278</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>1.06765</v>
+      </c>
       <c r="B32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>1.06765</v>
-      </c>
-      <c r="B35" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -963,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
@@ -977,25 +953,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <f>50+1614</f>
@@ -1008,7 +984,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <f>972+4013</f>
@@ -1021,7 +997,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <f>3955+13315</f>
@@ -1034,7 +1010,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <f>2879+2953</f>
@@ -1047,7 +1023,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <f>6236+2826</f>
@@ -1060,7 +1036,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <f>2156+2707</f>
@@ -1073,7 +1049,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <f>2918+12457</f>
@@ -1086,7 +1062,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <f>15095+29814</f>
@@ -1099,7 +1075,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <f>10315+29977</f>
@@ -1112,7 +1088,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1120,31 +1096,31 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <f>39/10</f>
@@ -1157,7 +1133,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>95.55</v>
@@ -1166,12 +1142,12 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>44.67</v>
@@ -1181,12 +1157,12 @@
         <v>13.041950354609931</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>58.48</v>
@@ -1197,12 +1173,12 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <f>21.5/10</f>
@@ -1215,7 +1191,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>65.11</v>
@@ -1224,12 +1200,12 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>50.76</v>
@@ -1240,7 +1216,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>58.48</v>
@@ -1251,12 +1227,12 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B26">
         <f>21.61/10</f>
@@ -1269,7 +1245,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B27">
         <v>65.11</v>
@@ -1278,12 +1254,12 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B28">
         <v>50.76</v>
@@ -1294,7 +1270,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>58.48</v>
@@ -1305,12 +1281,12 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <f>24.49/10</f>
@@ -1323,7 +1299,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B32" s="8">
         <f>AVERAGE(B27,B22,B17)</f>
@@ -1334,12 +1310,12 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B33" s="7">
         <f t="shared" ref="B33:C34" si="0">AVERAGE(B28,B23,B18)</f>
@@ -1350,12 +1326,12 @@
         <v>14.227316784869977</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B34" s="7">
         <f t="shared" si="0"/>
@@ -1366,17 +1342,17 @@
         <v>58.48</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1387,16 +1363,16 @@
         <v>177.68697307584281</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
-        <f>A39*About!A27</f>
+        <f>A39*About!A24</f>
         <v>227.08395159092711</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1429,12 +1405,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3">
         <f>'Forest Mgmt Costs'!A40</f>
@@ -1443,7 +1419,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
         <f>'Forest Mgmt Costs'!A40</f>
@@ -1452,7 +1428,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4" s="6">
         <v>0</v>
@@ -1460,7 +1436,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3">
         <f>'Forest Mgmt Costs'!A40</f>
@@ -1469,7 +1445,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -1477,10 +1453,11 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3">
-        <v>0</v>
+        <f>'Forest Mgmt Costs'!A40</f>
+        <v>227.08395159092711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>